<commit_message>
Can now run optimiser with relative weight
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B04897D-65BB-49CF-A325-5D0129AD2444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14404AAF-3C1E-4C64-8C13-E178DEC0AF83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" activeTab="2" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
+    <workbookView xWindow="14642" yWindow="2961" windowWidth="19380" windowHeight="10147" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
   <sheets>
     <sheet name="randomCalculations" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="vanderHoek" sheetId="4" r:id="rId4"/>
     <sheet name="realData" sheetId="5" r:id="rId5"/>
     <sheet name="verifyPoli" sheetId="7" r:id="rId6"/>
+    <sheet name="compOptGebradd" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="59">
   <si>
     <t>baseline control</t>
   </si>
@@ -201,6 +202,18 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>T number</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>optimised</t>
   </si>
 </sst>
 </file>
@@ -7638,6 +7651,413 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$5:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1855.61590285229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>917.74235268904101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>714.70070088930504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>656.45493639253402</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>638.07968558066602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4782.5935784038356</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B02-48CA-BDC8-7DCFE7F47E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$D$5:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1721.78240840125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>976.95631979742097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>896.46959680438704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>877.64282711932594</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>987.01070888513698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5459.8618610075218</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B02-48CA-BDC8-7DCFE7F47E56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="514651256"/>
+        <c:axId val="514656376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="514651256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Turbine</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514656376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="514656376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Power </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>[MW]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="514651256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -11435,9 +11855,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -13795,6 +14213,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -18224,6 +18682,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -22979,6 +23940,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76913</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>59820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>418744</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>68366</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F59C4384-938C-45FF-BF15-6D9129EDE4DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -24234,7 +25236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF65D761-B97A-44D4-B52B-D91498842DFD}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -25298,8 +26300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A22E781-0739-4923-86AD-A6E0286D2954}">
   <dimension ref="C2:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -28054,4 +29056,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
+  <dimension ref="B3:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1855.61590285229</v>
+      </c>
+      <c r="D5">
+        <v>1721.78240840125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>917.74235268904101</v>
+      </c>
+      <c r="D6">
+        <v>976.95631979742097</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>714.70070088930504</v>
+      </c>
+      <c r="D7">
+        <v>896.46959680438704</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>656.45493639253402</v>
+      </c>
+      <c r="D8">
+        <v>877.64282711932594</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>638.07968558066602</v>
+      </c>
+      <c r="D9">
+        <v>987.01070888513698</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <f>SUM(C5:C9)</f>
+        <v>4782.5935784038356</v>
+      </c>
+      <c r="D10">
+        <f>SUM(D5:D9)</f>
+        <v>5459.8618610075218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed optimiser, cost funcs are now relative to baseline
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14404AAF-3C1E-4C64-8C13-E178DEC0AF83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72E51A-6F6C-4692-B347-5E089A674E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14642" yWindow="2961" windowWidth="19380" windowHeight="10147" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
   <sheets>
     <sheet name="randomCalculations" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="realData" sheetId="5" r:id="rId5"/>
     <sheet name="verifyPoli" sheetId="7" r:id="rId6"/>
     <sheet name="compOptGebradd" sheetId="8" r:id="rId7"/>
+    <sheet name="FAST10ATCtU" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="62">
   <si>
     <t>baseline control</t>
   </si>
@@ -214,6 +215,15 @@
   </si>
   <si>
     <t>optimised</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Gebraad: FLORIS</t>
   </si>
 </sst>
 </file>
@@ -7712,105 +7722,348 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Baseline</c:v>
+            <c:v>FASTnAT baseline</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>compOptGebradd!$C$5:$C$10</c:f>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1855.61590285229</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>917.74235268904101</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>714.70070088930504</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>656.45493639253402</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>638.07968558066602</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4782.5935784038356</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.8556159028522901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91774235268904103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71470070088930504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65645493639253405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63807968558066608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5B02-48CA-BDC8-7DCFE7F47E56}"/>
+              <c16:uniqueId val="{00000000-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>FLORIS baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.8009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.622</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Optimised</c:v>
+            <c:v>FASTnAT optimised</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>compOptGebradd!$D$5:$D$10</c:f>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1721.78240840125</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>976.95631979742097</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>896.46959680438704</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>877.64282711932594</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>987.01070888513698</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5459.8618610075218</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.7217824084012501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97695631979742092</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89646959680438709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87764282711932595</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98701070888513698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5B02-48CA-BDC8-7DCFE7F47E56}"/>
+              <c16:uniqueId val="{00000001-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>FASTnAT optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$F$5:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.5669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97199999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7822,18 +8075,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="514651256"/>
-        <c:axId val="514656376"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="514651256"/>
+        <c:axId val="521064656"/>
+        <c:axId val="521062416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="521064656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -7856,7 +8123,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Turbine</a:t>
+                  <a:t>Turbine number</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7887,6 +8154,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7895,8 +8163,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -7920,7 +8188,403 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="514656376"/>
+        <c:crossAx val="521062416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="521062416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> Power</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> [MW]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521064656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>FASTnAT optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.7825935784038354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-00E2-467B-B1EB-CF8E37BC7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>FASTnAT optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.4598618610075222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-00E2-467B-B1EB-CF8E37BC7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FLORIS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.9119999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-00E2-467B-B1EB-CF8E37BC7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>FLORIS optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent6"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.883</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-00E2-467B-B1EB-CF8E37BC7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="468678904"/>
+        <c:axId val="468681144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="468678904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="468681144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7928,7 +8592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="514656376"/>
+        <c:axId val="468681144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7970,24 +8634,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Power </a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1100">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>[MW]</a:t>
+                  <a:t>Power [MW]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8046,7 +8693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="514651256"/>
+        <c:crossAx val="468678904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8058,6 +8705,34 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -8074,12 +8749,729 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Thrust coefficient</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>FAST10ATCtU!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>FAST10ATCtU!$D$5:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.77315300204195503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81470379225109002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82737163885901499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.830530057232446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83126807411625203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.831440084447851</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83148140059931397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83149062454432898</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83149282465894303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83149308952915602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6FA0-489F-BE55-602FE0D2F29F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="533159120"/>
+        <c:axId val="533155920"/>
+      </c:lineChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Wind speed at turbine</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FAST10ATCtU!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FAST10ATCtU!$C$5:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7678780082193901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.49380858657549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4299350750433097</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4152202865608201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.41180371542419</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4109850197613998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4108016451224099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.4107580423153001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4107525501072598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FA0-489F-BE55-602FE0D2F29F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="533178320"/>
+        <c:axId val="533178000"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="533159120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Turbine number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533155920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533155920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.85000000000000009"/>
+          <c:min val="0.75000000000000011"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Thrust</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> coefficient</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533159120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="2.0000000000000004E-2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533178000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
+          <c:min val="5.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Wind</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> speed [m/s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533178320"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="533178320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="533178000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -14253,6 +15645,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -18702,7 +20174,7 @@
 </file>
 
 <file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -18729,8 +20201,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -18831,7 +20303,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -18863,6 +20335,522 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -19185,6 +21173,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -23944,23 +26448,100 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76913</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>59820</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>128184</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>51275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>418744</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>68366</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>606751</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>170916</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFD3C599-0065-49B7-887C-2285CC2D44FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>8546</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>136732</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>136734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9FF1E62-1989-41A0-B7C9-0115EF4CC731}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25638</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>145278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>59821</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76913</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F59C4384-938C-45FF-BF15-6D9129EDE4DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83EBF558-837D-41ED-9243-A2D49FCA6150}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26534,7 +29115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F248FD9-301D-457F-AE14-7A8D9661D287}">
   <dimension ref="A2:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="U3" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AY34" sqref="AY34"/>
     </sheetView>
   </sheetViews>
@@ -29026,6 +31607,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="L18:T18"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
     <mergeCell ref="L2:T2"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="B33:J33"/>
@@ -29042,16 +31633,6 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="L33:T33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="L18:T18"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="R19:T19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -29060,27 +31641,234 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
-  <dimension ref="B3:D10"/>
+  <dimension ref="B3:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="13"/>
     </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>B12/1000</f>
+        <v>1.8556159028522901</v>
+      </c>
+      <c r="D5">
+        <f>C12/1000</f>
+        <v>1.7217824084012501</v>
+      </c>
+      <c r="E5">
+        <v>1.8009999999999999</v>
+      </c>
+      <c r="F5">
+        <v>1.5669999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D10" si="0">B13/1000</f>
+        <v>0.91774235268904103</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.97695631979742092</v>
+      </c>
+      <c r="E6">
+        <v>0.622</v>
+      </c>
+      <c r="F6">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.71470070088930504</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.89646959680438709</v>
+      </c>
+      <c r="E7">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.65645493639253405</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.87764282711932595</v>
+      </c>
+      <c r="E8">
+        <v>0.505</v>
+      </c>
+      <c r="F8">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.63807968558066608</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.98701070888513698</v>
+      </c>
+      <c r="E9">
+        <v>0.505</v>
+      </c>
+      <c r="F9">
+        <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.7825935784038354</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>5.4598618610075222</v>
+      </c>
+      <c r="E10">
+        <v>3.9119999999999999</v>
+      </c>
+      <c r="F10">
+        <v>4.883</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1855.61590285229</v>
+      </c>
+      <c r="C12">
+        <v>1721.78240840125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>917.74235268904101</v>
+      </c>
+      <c r="C13">
+        <v>976.95631979742097</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>714.70070088930504</v>
+      </c>
+      <c r="C14">
+        <v>896.46959680438704</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>656.45493639253402</v>
+      </c>
+      <c r="C15">
+        <v>877.64282711932594</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>638.07968558066602</v>
+      </c>
+      <c r="C16">
+        <v>987.01070888513698</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>SUM(B12:B16)</f>
+        <v>4782.5935784038356</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C12:C16)</f>
+        <v>5459.8618610075218</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74ABE64-0348-4EA8-A7AC-C6738F892931}">
+  <dimension ref="B4:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
+  <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -29088,10 +31876,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1855.61590285229</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>1721.78240840125</v>
+        <v>0.77315300204195503</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -29099,10 +31887,10 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>917.74235268904101</v>
+        <v>6.7678780082193901</v>
       </c>
       <c r="D6">
-        <v>976.95631979742097</v>
+        <v>0.81470379225109002</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -29110,10 +31898,10 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>714.70070088930504</v>
+        <v>6.49380858657549</v>
       </c>
       <c r="D7">
-        <v>896.46959680438704</v>
+        <v>0.82737163885901499</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -29121,10 +31909,10 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>656.45493639253402</v>
+        <v>6.4299350750433097</v>
       </c>
       <c r="D8">
-        <v>877.64282711932594</v>
+        <v>0.830530057232446</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -29132,23 +31920,65 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>638.07968558066602</v>
+        <v>6.4152202865608201</v>
       </c>
       <c r="D9">
-        <v>987.01070888513698</v>
+        <v>0.83126807411625203</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>56</v>
+      <c r="B10">
+        <v>6</v>
       </c>
       <c r="C10">
-        <f>SUM(C5:C9)</f>
-        <v>4782.5935784038356</v>
+        <v>6.41180371542419</v>
       </c>
       <c r="D10">
-        <f>SUM(D5:D9)</f>
-        <v>5459.8618610075218</v>
+        <v>0.831440084447851</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>6.4109850197613998</v>
+      </c>
+      <c r="D11">
+        <v>0.83148140059931397</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>6.4108016451224099</v>
+      </c>
+      <c r="D12">
+        <v>0.83149062454432898</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>6.4107580423153001</v>
+      </c>
+      <c r="D13">
+        <v>0.83149282465894303</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>6.4107525501072598</v>
+      </c>
+      <c r="D14">
+        <v>0.83149308952915602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved some scripts around, so they can be saved to github.
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E72E51A-6F6C-4692-B347-5E089A674E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7872000-F6B4-4066-8A57-C5717E7C796F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="5" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
   <sheets>
     <sheet name="randomCalculations" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1524,40 +1526,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.11414821113035</c:v>
+                  <c:v>1.11282245532541</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99102631401959096</c:v>
+                  <c:v>0.98813021058449002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90236688751309901</c:v>
+                  <c:v>0.90829385876831203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84196411012810801</c:v>
+                  <c:v>0.84850212610210696</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80361216038184902</c:v>
+                  <c:v>0.80274229166033695</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78389732249055699</c:v>
+                  <c:v>0.77731689390243597</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78110521679155698</c:v>
+                  <c:v>0.774040939958625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76823745787446496</c:v>
+                  <c:v>0.76470471354569702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75880306214780502</c:v>
+                  <c:v>0.76656106559533899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75402425525037198</c:v>
+                  <c:v>0.76446638636153996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74659620812881</c:v>
+                  <c:v>0.75119901249830001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.73954707418721999</c:v>
+                  <c:v>0.72838039770474206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1651,40 +1653,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.11812394184467</c:v>
+                  <c:v>1.11649662735674</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99443960027638301</c:v>
+                  <c:v>0.99177936348096696</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90527766816105604</c:v>
+                  <c:v>0.91141454551685497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84443232401592205</c:v>
+                  <c:v>0.85099278349674801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80569774635821401</c:v>
+                  <c:v>0.80475172660941297</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78570782176357401</c:v>
+                  <c:v>0.77911385555199697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78286811370516596</c:v>
+                  <c:v>0.77581681579196404</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.76973760457400997</c:v>
+                  <c:v>0.76644203632181196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.760100397481979</c:v>
+                  <c:v>0.76825067040861295</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75524988051951603</c:v>
+                  <c:v>0.76604231103809906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74775067094630698</c:v>
+                  <c:v>0.752476049786164</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.74066117087567995</c:v>
+                  <c:v>0.729281728534658</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1778,40 +1780,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.12209967255899</c:v>
+                  <c:v>1.1201707993880601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99785288653317505</c:v>
+                  <c:v>0.99542851637744401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90818844880901195</c:v>
+                  <c:v>0.91453523226540101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84690053790373598</c:v>
+                  <c:v>0.85348344089139005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.807783332334579</c:v>
+                  <c:v>0.80676116155848598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78751832103659103</c:v>
+                  <c:v>0.78091081720155997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78463101061877405</c:v>
+                  <c:v>0.77759269162530698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77123775127355498</c:v>
+                  <c:v>0.768179359097929</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76139773281615397</c:v>
+                  <c:v>0.76994027522188002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.75647550578865996</c:v>
+                  <c:v>0.76761823571465204</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74890513376380397</c:v>
+                  <c:v>0.75375308707402</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.74177526756413903</c:v>
+                  <c:v>0.73018305936456596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2565,37 +2567,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>177.80563192530701</c:v>
+                  <c:v>174.37340371282701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>402.14431192913798</c:v>
+                  <c:v>402.61320821931503</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>725.98379631410296</c:v>
+                  <c:v>723.840633671467</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1166.4004629032199</c:v>
+                  <c:v>1155.96430182483</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1638.93411403871</c:v>
+                  <c:v>1622.4493617687999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1740.4706895195</c:v>
+                  <c:v>1723.3413143221901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2465.27085398596</c:v>
+                  <c:v>2449.2130137742602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3357.8773341256101</c:v>
+                  <c:v>3348.1407448404202</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3818.8468480930501</c:v>
+                  <c:v>3809.4556894782399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4435.3665077614696</c:v>
+                  <c:v>4418.4416153094398</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4921.9544400271097</c:v>
+                  <c:v>4889.8091686149701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2686,37 +2688,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>177.72325560438401</c:v>
+                  <c:v>174.471248039523</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>403.81123535391202</c:v>
+                  <c:v>403.82204766932603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>729.85400705665802</c:v>
+                  <c:v>725.371047897067</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1172.9279485356401</c:v>
+                  <c:v>1157.9362050827499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1648.04455217432</c:v>
+                  <c:v>1625.32190847437</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1750.1094376138601</c:v>
+                  <c:v>1726.45912987207</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>2478.4748521143501</c:v>
+                  <c:v>2454.44084827712</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3375.1005698601198</c:v>
+                  <c:v>3356.3775627571299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3838.0268541957098</c:v>
+                  <c:v>3819.2478350770298</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4457.0629686741804</c:v>
+                  <c:v>4430.1964132991498</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4945.5673075312798</c:v>
+                  <c:v>4902.9644781163397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2810,40 +2812,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>33.136001490524201</c:v>
+                  <c:v>29.151854502294501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>177.640879283461</c:v>
+                  <c:v>174.569092366219</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>405.47815877868601</c:v>
+                  <c:v>405.03088711933702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>733.72421779921206</c:v>
+                  <c:v>726.901462122667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1179.45543416806</c:v>
+                  <c:v>1159.90810834067</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1657.1549903099401</c:v>
+                  <c:v>1628.1944551799299</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1759.74818570823</c:v>
+                  <c:v>1729.5769454219401</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2491.6788502427498</c:v>
+                  <c:v>2459.6686827799799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3392.3238055946299</c:v>
+                  <c:v>3364.6143806738301</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3857.20686029836</c:v>
+                  <c:v>3829.0399806758201</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4478.7594295868903</c:v>
+                  <c:v>4441.9512112888697</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4969.1801750354498</c:v>
+                  <c:v>4916.1197876177102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3566,37 +3568,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>780.148474098169</c:v>
+                  <c:v>785.74329669606698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>705.74621663434698</c:v>
+                  <c:v>717.29267704757899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>671.94936825949605</c:v>
+                  <c:v>678.08874513839805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>674.22275247926405</c:v>
+                  <c:v>672.43753796802002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>700.68960841254398</c:v>
+                  <c:v>695.43945437145805</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>708.03119279929604</c:v>
+                  <c:v>702.68335255373495</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>768.83951272524098</c:v>
+                  <c:v>767.12069253163702</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>852.11253576274805</c:v>
+                  <c:v>857.90621475764499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>895.70616443255801</c:v>
+                  <c:v>903.42848469036505</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>953.31508541746098</c:v>
+                  <c:v>958.97067590851998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>997.80049319743</c:v>
+                  <c:v>996.75898384619995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3687,37 +3689,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>785.25018372940201</c:v>
+                  <c:v>795.870169128322</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>724.13115926147304</c:v>
+                  <c:v>735.97384496628194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>709.00768326535001</c:v>
+                  <c:v>711.24552705841904</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>735.344579246683</c:v>
+                  <c:v>729.34936148879501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>786.19028477473603</c:v>
+                  <c:v>779.94481340254094</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>798.60667071111902</c:v>
+                  <c:v>793.156312641005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>894.25878116430397</c:v>
+                  <c:v>898.65610979919302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1017.76573411189</c:v>
+                  <c:v>1032.8691937490601</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1081.2231642148799</c:v>
+                  <c:v>1096.6863293025999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1164.5923530595101</c:v>
+                  <c:v>1171.7586633789001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1228.83662758384</c:v>
+                  <c:v>1220.78439795182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3811,40 +3813,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>894.10854918167104</c:v>
+                  <c:v>881.86956981683795</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>790.35189336063604</c:v>
+                  <c:v>805.99704156057601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>742.51610188859695</c:v>
+                  <c:v>754.65501288498604</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>746.06599827120397</c:v>
+                  <c:v>744.40230897844003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>796.46640601410297</c:v>
+                  <c:v>786.26118500956898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>871.69096113692694</c:v>
+                  <c:v>864.45017243362599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>889.18214862294099</c:v>
+                  <c:v>883.62927272827505</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1019.67804960337</c:v>
+                  <c:v>1030.19152706675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1183.41893246103</c:v>
+                  <c:v>1207.83217274048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1266.7401639972099</c:v>
+                  <c:v>1289.9441739148399</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1375.8696207015701</c:v>
+                  <c:v>1384.54665084928</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1459.8727619702599</c:v>
+                  <c:v>1444.80981205744</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4550,37 +4552,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.70840355356234097</c:v>
+                  <c:v>0.71554379249597699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69179921623726404</c:v>
+                  <c:v>0.69969052049724501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67325227011894195</c:v>
+                  <c:v>0.67332800944378501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65453096290609203</c:v>
+                  <c:v>0.64772178559601201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63996394031786397</c:v>
+                  <c:v>0.63293325637311704</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63740354229742902</c:v>
+                  <c:v>0.63105598561667398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.623638255991671</c:v>
+                  <c:v>0.62582215575492595</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.61500335168753495</c:v>
+                  <c:v>0.62620805103041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61326255937492902</c:v>
+                  <c:v>0.624224255061815</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61326707708373596</c:v>
+                  <c:v>0.61548643441733097</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.61490027104282396</c:v>
+                  <c:v>0.60182505694496402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4660,37 +4662,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.708333932537075</c:v>
+                  <c:v>0.71667825372239002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69229806243879299</c:v>
+                  <c:v>0.70109668414573101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67414781889175501</c:v>
+                  <c:v>0.67471139301703398</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65565144959467603</c:v>
+                  <c:v>0.64888723133800297</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.64114063512991704</c:v>
+                  <c:v>0.63384346815953496</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.63857720224627401</c:v>
+                  <c:v>0.63191618560031304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.62469332454526605</c:v>
+                  <c:v>0.62640617696969203</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.615768064190367</c:v>
+                  <c:v>0.62666986046999695</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61384057343605802</c:v>
+                  <c:v>0.62471653806425997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61356966888029596</c:v>
+                  <c:v>0.61611342416729298</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.61496992045333099</c:v>
+                  <c:v>0.60263009900029496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4773,40 +4775,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.71967732858031097</c:v>
+                  <c:v>0.71010706370459398</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70826431151180902</c:v>
+                  <c:v>0.71781271494880206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69279690864032195</c:v>
+                  <c:v>0.70250284779421601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67504336766456696</c:v>
+                  <c:v>0.67609477659028405</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65677193628326003</c:v>
+                  <c:v>0.65005267707999403</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64231732994197099</c:v>
+                  <c:v>0.634753679945953</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63975086219511901</c:v>
+                  <c:v>0.632776385583951</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62574839309885999</c:v>
+                  <c:v>0.626990198184457</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61653277669319995</c:v>
+                  <c:v>0.62713166990958402</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61441858749718803</c:v>
+                  <c:v>0.62520882106670395</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.61387226067685496</c:v>
+                  <c:v>0.61674041391725698</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.61503956986383801</c:v>
+                  <c:v>0.60343514105562801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5488,31 +5490,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>542.97273045320605</c:v>
+                  <c:v>547.74428273313004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>935.38851030200703</c:v>
+                  <c:v>915.41586116505198</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1325.3713084456001</c:v>
+                  <c:v>1315.9694171757501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1407.61169182147</c:v>
+                  <c:v>1399.75506398316</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1991.7079034202</c:v>
+                  <c:v>1984.33473978302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2719.7427735067999</c:v>
+                  <c:v>2705.7889454477099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3102.8619382465399</c:v>
+                  <c:v>3087.64941081298</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3623.7819304898499</c:v>
+                  <c:v>3607.8353828376798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4041.8614943776001</c:v>
+                  <c:v>4022.65764120943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5591,25 +5593,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1328.92674706194</c:v>
+                  <c:v>1316.7708608599301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1411.5586272595799</c:v>
+                  <c:v>1400.4216975235299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1999.5889810016699</c:v>
+                  <c:v>1985.5279015040101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2734.12228117528</c:v>
+                  <c:v>2711.6754470974101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3121.00233839579</c:v>
+                  <c:v>3097.3037538869398</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3647.22415618899</c:v>
+                  <c:v>3623.4003246114298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4069.6468079132301</c:v>
+                  <c:v>4043.2656580462499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5688,25 +5690,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1332.4821856782901</c:v>
+                  <c:v>1317.57230454413</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1415.50556269769</c:v>
+                  <c:v>1401.0883310639199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2007.4700585831399</c:v>
+                  <c:v>1986.7210632250101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2748.5017888437601</c:v>
+                  <c:v>2717.5619487471099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3139.1427385450402</c:v>
+                  <c:v>3106.9580969608801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3670.6663818881302</c:v>
+                  <c:v>3638.9652663851698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4097.43212144886</c:v>
+                  <c:v>4063.8736748830902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6357,31 +6359,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>762.53360427435803</c:v>
+                  <c:v>753.20727953816004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>712.78611359517004</c:v>
+                  <c:v>719.76948328114395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>715.30282426629799</c:v>
+                  <c:v>723.02584877542495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>719.545634031605</c:v>
+                  <c:v>726.31053133697196</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>767.381637354497</c:v>
+                  <c:v>765.77408876231505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>840.86359533468396</c:v>
+                  <c:v>837.12421420181101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>878.18619776765104</c:v>
+                  <c:v>877.34892526303304</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>924.56097974299701</c:v>
+                  <c:v>928.75403707374596</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>957.44381458286705</c:v>
+                  <c:v>963.691728248392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6460,25 +6462,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>784.76961933794405</c:v>
+                  <c:v>789.32023149388999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>794.35080565490898</c:v>
+                  <c:v>797.57689773783</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>877.45761182013405</c:v>
+                  <c:v>874.66968974920201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>989.49649228828002</c:v>
+                  <c:v>991.53582019791395</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1045.24180637521</c:v>
+                  <c:v>1051.63709549177</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1115.03691883018</c:v>
+                  <c:v>1123.12313692978</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1165.5770840242601</c:v>
+                  <c:v>1167.37795444631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6557,25 +6559,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>854.23641440958795</c:v>
+                  <c:v>855.61461421236004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>869.15597727821205</c:v>
+                  <c:v>868.84326413867598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>987.53358628576996</c:v>
+                  <c:v>983.56529073606498</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1138.1293892418801</c:v>
+                  <c:v>1145.9474261939999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1212.2974149827801</c:v>
+                  <c:v>1225.92526572051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1305.51285791736</c:v>
+                  <c:v>1317.4922367858101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1373.7103534656501</c:v>
+                  <c:v>1371.0641806441699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7256,31 +7258,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.46580861379627098</c:v>
+                  <c:v>0.46543611916955102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46996278912905798</c:v>
+                  <c:v>0.471107339540415</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47134135109165498</c:v>
+                  <c:v>0.47141842532749301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47141239352936098</c:v>
+                  <c:v>0.47129689042422201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47066336887219001</c:v>
+                  <c:v>0.47015533861462899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46822165703255397</c:v>
+                  <c:v>0.46851708987673102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46670544939976</c:v>
+                  <c:v>0.467307760547436</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46459319988546</c:v>
+                  <c:v>0.46502335969716502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46292285932053701</c:v>
+                  <c:v>0.46257253765678902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7359,25 +7361,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.47097373719661401</c:v>
+                  <c:v>0.47121053665513002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47101418687577101</c:v>
+                  <c:v>0.471055323404309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47027155534312798</c:v>
+                  <c:v>0.469826841231412</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46817692260295102</c:v>
+                  <c:v>0.46847802052781901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46692804936423699</c:v>
+                  <c:v>0.46754861624806898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46523623053024998</c:v>
+                  <c:v>0.465724491972133</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46393638806806398</c:v>
+                  <c:v>0.46367589977865298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7456,25 +7458,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.47060612330157298</c:v>
+                  <c:v>0.47100264798276797</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47061598022217999</c:v>
+                  <c:v>0.47081375638439599</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.469879741814066</c:v>
+                  <c:v>0.469498343848194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46813218817334901</c:v>
+                  <c:v>0.46843895117890799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46715064932871297</c:v>
+                  <c:v>0.46778947194870102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46587926117503897</c:v>
+                  <c:v>0.46642562424710099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.464949916815591</c:v>
+                  <c:v>0.46477926190051699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7564,6 +7566,7 @@
         <c:axId val="432975800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7957,19 +7960,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.7217824084012501</c:v>
+                  <c:v>1.8010977482444401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97695631979742092</c:v>
+                  <c:v>1.0131010128053801</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89646959680438709</c:v>
+                  <c:v>0.85670654653141298</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.87764282711932595</c:v>
+                  <c:v>0.81876682645388499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98701070888513698</c:v>
+                  <c:v>0.80387616088661606</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8477,7 +8480,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.4598618610075222</c:v>
+                  <c:v>5.2935482949217336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13810,40 +13813,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>30.4700429854893</c:v>
+                  <c:v>31.583809572398799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175.01006813125599</c:v>
+                  <c:v>171.06243280021999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>412.92151668878398</c:v>
+                  <c:v>407.37192871235698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>762.29314700191605</c:v>
+                  <c:v>756.78866796187106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1241.2137174145</c:v>
+                  <c:v>1234.88665879155</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1756.85586365414</c:v>
+                  <c:v>1747.69382110418</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1867.77198627037</c:v>
+                  <c:v>1857.80190202887</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2660.0567119133698</c:v>
+                  <c:v>2643.4967460809398</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3636.1566526873498</c:v>
+                  <c:v>3613.02424192947</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4140.1908635233603</c:v>
+                  <c:v>4115.8651817259697</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4814.1605669361597</c:v>
+                  <c:v>4791.7924981257402</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5345.9471270776503</c:v>
+                  <c:v>5328.6196779864504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13937,40 +13940,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>28.184673424029299</c:v>
+                  <c:v>29.124452665336602</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175.44597144302199</c:v>
+                  <c:v>171.772857160217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>416.04651777056898</c:v>
+                  <c:v>408.79461393043402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>768.07507075051296</c:v>
+                  <c:v>758.42479277888503</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1249.6203887267</c:v>
+                  <c:v>1237.3902334014699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1767.44245800001</c:v>
+                  <c:v>1751.7088881472901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1878.77123004297</c:v>
+                  <c:v>1862.1739003820201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2673.61635304316</c:v>
+                  <c:v>2650.2792381873201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3652.24451607113</c:v>
+                  <c:v>3621.49452616198</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4157.4059297940103</c:v>
+                  <c:v>4124.3370181308801</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4832.7444774707101</c:v>
+                  <c:v>4799.1572335234696</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5365.5204474436196</c:v>
+                  <c:v>5334.1427979609798</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14064,40 +14067,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>25.899303862569202</c:v>
+                  <c:v>26.665095758274401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175.88187475478799</c:v>
+                  <c:v>172.48328152021301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>419.17151885235501</c:v>
+                  <c:v>410.21729914850999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>773.85699449911101</c:v>
+                  <c:v>760.06091759589901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1258.0270600388999</c:v>
+                  <c:v>1239.8938080113801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1778.02905234588</c:v>
+                  <c:v>1755.7239551904099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1889.7704738155701</c:v>
+                  <c:v>1866.5458987351799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2687.1759941729601</c:v>
+                  <c:v>2657.0617302936998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3668.3323794549101</c:v>
+                  <c:v>3629.9648103944901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4174.6209960646602</c:v>
+                  <c:v>4132.8088545357896</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4851.3283880052704</c:v>
+                  <c:v>4806.5219689211899</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5385.0937678095897</c:v>
+                  <c:v>5339.6659179355001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14788,40 +14791,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>825.30161285013503</c:v>
+                  <c:v>810.09718011994005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>703.16797265105799</c:v>
+                  <c:v>711.49863675317499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>638.87221443493604</c:v>
+                  <c:v>654.414955370999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>623.94503334092303</c:v>
+                  <c:v>633.69637673368595</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>649.91712450817101</c:v>
+                  <c:v>648.96531883032696</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>697.14463076484503</c:v>
+                  <c:v>689.907803143141</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>708.31918307583396</c:v>
+                  <c:v>700.54200248679899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>790.68190418306494</c:v>
+                  <c:v>785.37007697376896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>888.535982969016</c:v>
+                  <c:v>892.94224561466604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>935.36783345151503</c:v>
+                  <c:v>943.42489182239399</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>993.41211457284203</c:v>
+                  <c:v>1001.22589139365</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1035.4316177145499</c:v>
+                  <c:v>1036.92616652164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14904,40 +14907,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>825.87462210368301</c:v>
+                  <c:v>813.88498323912097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>715.80644742528204</c:v>
+                  <c:v>726.97686573130204</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>668.247283183219</c:v>
+                  <c:v>681.37398976286602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>674.72782451664705</c:v>
+                  <c:v>678.40274043389604</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>726.77876656471904</c:v>
+                  <c:v>720.94098002936096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>799.522355630059</c:v>
+                  <c:v>792.267918102458</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>815.93080446658905</c:v>
+                  <c:v>809.34367362710395</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>933.714633361408</c:v>
+                  <c:v>937.36851470581996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1071.6609483883301</c:v>
+                  <c:v>1088.1015507530401</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1138.0582608371799</c:v>
+                  <c:v>1155.5477774015001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1221.30044468651</c:v>
+                  <c:v>1229.88280887313</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1282.5332096729001</c:v>
+                  <c:v>1273.5066685138599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15020,40 +15023,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>826.44763135723099</c:v>
+                  <c:v>817.67278635830303</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>728.44492219950598</c:v>
+                  <c:v>742.45509470943</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>697.62235193150195</c:v>
+                  <c:v>708.33302415473395</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>725.51061569237095</c:v>
+                  <c:v>723.10910413410602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>803.64040862126797</c:v>
+                  <c:v>792.916641228397</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>901.90008049527296</c:v>
+                  <c:v>894.62803306177602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>923.54242585734301</c:v>
+                  <c:v>918.14534476740596</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1076.7473625397499</c:v>
+                  <c:v>1089.3669524378699</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1254.7859138076501</c:v>
+                  <c:v>1283.2608558914201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1340.74868822285</c:v>
+                  <c:v>1367.6706629805999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1449.18877480018</c:v>
+                  <c:v>1458.5397263526099</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1529.63480163126</c:v>
+                  <c:v>1510.0871705060799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -29115,8 +29118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F248FD9-301D-457F-AE14-7A8D9661D287}">
   <dimension ref="A2:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AY34" sqref="AY34"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36:T47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -29289,31 +29292,31 @@
         <v>1.11794826225293</v>
       </c>
       <c r="L6">
-        <v>30.4700429854893</v>
+        <v>31.583809572398799</v>
       </c>
       <c r="M6">
-        <v>825.30161285013503</v>
+        <v>810.09718011994005</v>
       </c>
       <c r="N6">
-        <v>1.11414821113035</v>
+        <v>1.11282245532541</v>
       </c>
       <c r="O6">
-        <v>28.184673424029299</v>
+        <v>29.124452665336602</v>
       </c>
       <c r="P6">
-        <v>825.87462210368301</v>
+        <v>813.88498323912097</v>
       </c>
       <c r="Q6">
-        <v>1.11812394184467</v>
+        <v>1.11649662735674</v>
       </c>
       <c r="R6">
-        <v>25.899303862569202</v>
+        <v>26.665095758274401</v>
       </c>
       <c r="S6">
-        <v>826.44763135723099</v>
+        <v>817.67278635830303</v>
       </c>
       <c r="T6">
-        <v>1.12209967255899</v>
+        <v>1.1201707993880601</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -29348,31 +29351,31 @@
         <v>0.99209620604398996</v>
       </c>
       <c r="L7">
-        <v>175.01006813125599</v>
+        <v>171.06243280021999</v>
       </c>
       <c r="M7">
-        <v>703.16797265105799</v>
+        <v>711.49863675317499</v>
       </c>
       <c r="N7">
-        <v>0.99102631401959096</v>
+        <v>0.98813021058449002</v>
       </c>
       <c r="O7">
-        <v>175.44597144302199</v>
+        <v>171.772857160217</v>
       </c>
       <c r="P7">
-        <v>715.80644742528204</v>
+        <v>726.97686573130204</v>
       </c>
       <c r="Q7">
-        <v>0.99443960027638301</v>
+        <v>0.99177936348096696</v>
       </c>
       <c r="R7">
-        <v>175.88187475478799</v>
+        <v>172.48328152021301</v>
       </c>
       <c r="S7">
-        <v>728.44492219950598</v>
+        <v>742.45509470943</v>
       </c>
       <c r="T7">
-        <v>0.99785288653317505</v>
+        <v>0.99542851637744401</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -29407,31 +29410,31 @@
         <v>0.91220101238397699</v>
       </c>
       <c r="L8">
-        <v>412.92151668878398</v>
+        <v>407.37192871235698</v>
       </c>
       <c r="M8">
-        <v>638.87221443493604</v>
+        <v>654.414955370999</v>
       </c>
       <c r="N8">
-        <v>0.90236688751309901</v>
+        <v>0.90829385876831203</v>
       </c>
       <c r="O8">
-        <v>416.04651777056898</v>
+        <v>408.79461393043402</v>
       </c>
       <c r="P8">
-        <v>668.247283183219</v>
+        <v>681.37398976286602</v>
       </c>
       <c r="Q8">
-        <v>0.90527766816105604</v>
+        <v>0.91141454551685497</v>
       </c>
       <c r="R8">
-        <v>419.17151885235501</v>
+        <v>410.21729914850999</v>
       </c>
       <c r="S8">
-        <v>697.62235193150195</v>
+        <v>708.33302415473395</v>
       </c>
       <c r="T8">
-        <v>0.90818844880901195</v>
+        <v>0.91453523226540101</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -29466,31 +29469,31 @@
         <v>0.85382927738603498</v>
       </c>
       <c r="L9">
-        <v>762.29314700191605</v>
+        <v>756.78866796187106</v>
       </c>
       <c r="M9">
-        <v>623.94503334092303</v>
+        <v>633.69637673368595</v>
       </c>
       <c r="N9">
-        <v>0.84196411012810801</v>
+        <v>0.84850212610210696</v>
       </c>
       <c r="O9">
-        <v>768.07507075051296</v>
+        <v>758.42479277888503</v>
       </c>
       <c r="P9">
-        <v>674.72782451664705</v>
+        <v>678.40274043389604</v>
       </c>
       <c r="Q9">
-        <v>0.84443232401592205</v>
+        <v>0.85099278349674801</v>
       </c>
       <c r="R9">
-        <v>773.85699449911101</v>
+        <v>760.06091759589901</v>
       </c>
       <c r="S9">
-        <v>725.51061569237095</v>
+        <v>723.10910413410602</v>
       </c>
       <c r="T9">
-        <v>0.84690053790373598</v>
+        <v>0.85348344089139005</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -29525,31 +29528,31 @@
         <v>0.80738682545164897</v>
       </c>
       <c r="L10">
-        <v>1241.2137174145</v>
+        <v>1234.88665879155</v>
       </c>
       <c r="M10">
-        <v>649.91712450817101</v>
+        <v>648.96531883032696</v>
       </c>
       <c r="N10">
-        <v>0.80361216038184902</v>
+        <v>0.80274229166033695</v>
       </c>
       <c r="O10">
-        <v>1249.6203887267</v>
+        <v>1237.3902334014699</v>
       </c>
       <c r="P10">
-        <v>726.77876656471904</v>
+        <v>720.94098002936096</v>
       </c>
       <c r="Q10">
-        <v>0.80569774635821401</v>
+        <v>0.80475172660941297</v>
       </c>
       <c r="R10">
-        <v>1258.0270600388999</v>
+        <v>1239.8938080113801</v>
       </c>
       <c r="S10">
-        <v>803.64040862126797</v>
+        <v>792.916641228397</v>
       </c>
       <c r="T10">
-        <v>0.807783332334579</v>
+        <v>0.80676116155848598</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -29584,31 +29587,31 @@
         <v>0.77472591656962497</v>
       </c>
       <c r="L11">
-        <v>1756.85586365414</v>
+        <v>1747.69382110418</v>
       </c>
       <c r="M11">
-        <v>697.14463076484503</v>
+        <v>689.907803143141</v>
       </c>
       <c r="N11">
-        <v>0.78389732249055699</v>
+        <v>0.77731689390243597</v>
       </c>
       <c r="O11">
-        <v>1767.44245800001</v>
+        <v>1751.7088881472901</v>
       </c>
       <c r="P11">
-        <v>799.522355630059</v>
+        <v>792.267918102458</v>
       </c>
       <c r="Q11">
-        <v>0.78570782176357401</v>
+        <v>0.77911385555199697</v>
       </c>
       <c r="R11">
-        <v>1778.02905234588</v>
+        <v>1755.7239551904099</v>
       </c>
       <c r="S11">
-        <v>901.90008049527296</v>
+        <v>894.62803306177602</v>
       </c>
       <c r="T11">
-        <v>0.78751832103659103</v>
+        <v>0.78091081720155997</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -29643,31 +29646,31 @@
         <v>0.77422469768903701</v>
       </c>
       <c r="L12">
-        <v>1867.77198627037</v>
+        <v>1857.80190202887</v>
       </c>
       <c r="M12">
-        <v>708.31918307583396</v>
+        <v>700.54200248679899</v>
       </c>
       <c r="N12">
-        <v>0.78110521679155698</v>
+        <v>0.774040939958625</v>
       </c>
       <c r="O12">
-        <v>1878.77123004297</v>
+        <v>1862.1739003820201</v>
       </c>
       <c r="P12">
-        <v>815.93080446658905</v>
+        <v>809.34367362710395</v>
       </c>
       <c r="Q12">
-        <v>0.78286811370516596</v>
+        <v>0.77581681579196404</v>
       </c>
       <c r="R12">
-        <v>1889.7704738155701</v>
+        <v>1866.5458987351799</v>
       </c>
       <c r="S12">
-        <v>923.54242585734301</v>
+        <v>918.14534476740596</v>
       </c>
       <c r="T12">
-        <v>0.78463101061877405</v>
+        <v>0.77759269162530698</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -29702,31 +29705,31 @@
         <v>0.77207115742542398</v>
       </c>
       <c r="L13">
-        <v>2660.0567119133698</v>
+        <v>2643.4967460809398</v>
       </c>
       <c r="M13">
-        <v>790.68190418306494</v>
+        <v>785.37007697376896</v>
       </c>
       <c r="N13">
-        <v>0.76823745787446496</v>
+        <v>0.76470471354569702</v>
       </c>
       <c r="O13">
-        <v>2673.61635304316</v>
+        <v>2650.2792381873201</v>
       </c>
       <c r="P13">
-        <v>933.714633361408</v>
+        <v>937.36851470581996</v>
       </c>
       <c r="Q13">
-        <v>0.76973760457400997</v>
+        <v>0.76644203632181196</v>
       </c>
       <c r="R13">
-        <v>2687.1759941729601</v>
+        <v>2657.0617302936998</v>
       </c>
       <c r="S13">
-        <v>1076.7473625397499</v>
+        <v>1089.3669524378699</v>
       </c>
       <c r="T13">
-        <v>0.77123775127355498</v>
+        <v>0.768179359097929</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -29761,31 +29764,31 @@
         <v>0.76939282070950299</v>
       </c>
       <c r="L14">
-        <v>3636.1566526873498</v>
+        <v>3613.02424192947</v>
       </c>
       <c r="M14">
-        <v>888.535982969016</v>
+        <v>892.94224561466604</v>
       </c>
       <c r="N14">
-        <v>0.75880306214780502</v>
+        <v>0.76656106559533899</v>
       </c>
       <c r="O14">
-        <v>3652.24451607113</v>
+        <v>3621.49452616198</v>
       </c>
       <c r="P14">
-        <v>1071.6609483883301</v>
+        <v>1088.1015507530401</v>
       </c>
       <c r="Q14">
-        <v>0.760100397481979</v>
+        <v>0.76825067040861295</v>
       </c>
       <c r="R14">
-        <v>3668.3323794549101</v>
+        <v>3629.9648103944901</v>
       </c>
       <c r="S14">
-        <v>1254.7859138076501</v>
+        <v>1283.2608558914201</v>
       </c>
       <c r="T14">
-        <v>0.76139773281615397</v>
+        <v>0.76994027522188002</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -29820,31 +29823,31 @@
         <v>0.76769404192719104</v>
       </c>
       <c r="L15">
-        <v>4140.1908635233603</v>
+        <v>4115.8651817259697</v>
       </c>
       <c r="M15" s="8">
-        <v>935.36783345151503</v>
+        <v>943.42489182239399</v>
       </c>
       <c r="N15" s="8">
-        <v>0.75402425525037198</v>
+        <v>0.76446638636153996</v>
       </c>
       <c r="O15" s="8">
-        <v>4157.4059297940103</v>
+        <v>4124.3370181308801</v>
       </c>
       <c r="P15">
-        <v>1138.0582608371799</v>
+        <v>1155.5477774015001</v>
       </c>
       <c r="Q15" s="8">
-        <v>0.75524988051951603</v>
+        <v>0.76604231103809906</v>
       </c>
       <c r="R15" s="8">
-        <v>4174.6209960646602</v>
+        <v>4132.8088545357896</v>
       </c>
       <c r="S15" s="8">
-        <v>1340.74868822285</v>
+        <v>1367.6706629805999</v>
       </c>
       <c r="T15">
-        <v>0.75647550578865996</v>
+        <v>0.76761823571465204</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -29879,31 +29882,31 @@
         <v>0.747403193906373</v>
       </c>
       <c r="L16">
-        <v>4814.1605669361597</v>
+        <v>4791.7924981257402</v>
       </c>
       <c r="M16">
-        <v>993.41211457284203</v>
+        <v>1001.22589139365</v>
       </c>
       <c r="N16">
-        <v>0.74659620812881</v>
+        <v>0.75119901249830001</v>
       </c>
       <c r="O16">
-        <v>4832.7444774707101</v>
+        <v>4799.1572335234696</v>
       </c>
       <c r="P16">
-        <v>1221.30044468651</v>
+        <v>1229.88280887313</v>
       </c>
       <c r="Q16">
-        <v>0.74775067094630698</v>
+        <v>0.752476049786164</v>
       </c>
       <c r="R16">
-        <v>4851.3283880052704</v>
+        <v>4806.5219689211899</v>
       </c>
       <c r="S16">
-        <v>1449.18877480018</v>
+        <v>1458.5397263526099</v>
       </c>
       <c r="T16">
-        <v>0.74890513376380397</v>
+        <v>0.75375308707402</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -29938,31 +29941,31 @@
         <v>0.73262692098478899</v>
       </c>
       <c r="L17">
-        <v>5345.9471270776503</v>
+        <v>5328.6196779864504</v>
       </c>
       <c r="M17">
-        <v>1035.4316177145499</v>
+        <v>1036.92616652164</v>
       </c>
       <c r="N17">
-        <v>0.73954707418721999</v>
+        <v>0.72838039770474206</v>
       </c>
       <c r="O17">
-        <v>5365.5204474436196</v>
+        <v>5334.1427979609798</v>
       </c>
       <c r="P17">
-        <v>1282.5332096729001</v>
+        <v>1273.5066685138599</v>
       </c>
       <c r="Q17">
-        <v>0.74066117087567995</v>
+        <v>0.729281728534658</v>
       </c>
       <c r="R17">
-        <v>5385.0937678095897</v>
+        <v>5339.6659179355001</v>
       </c>
       <c r="S17">
-        <v>1529.63480163126</v>
+        <v>1510.0871705060799</v>
       </c>
       <c r="T17">
-        <v>0.74177526756413903</v>
+        <v>0.73018305936456596</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -30109,31 +30112,31 @@
         <v>0.71090680388438499</v>
       </c>
       <c r="L21">
-        <v>35.891378479597897</v>
+        <v>35.225317202969798</v>
       </c>
       <c r="M21">
-        <v>899.69131714531295</v>
+        <v>879.26088050114004</v>
       </c>
       <c r="N21">
-        <v>0.72129703439545501</v>
+        <v>0.709152110397817</v>
       </c>
       <c r="O21">
-        <v>34.513689985061099</v>
+        <v>32.188585852632201</v>
       </c>
       <c r="P21">
-        <v>896.89993316349205</v>
+        <v>880.56522515898905</v>
       </c>
       <c r="Q21">
-        <v>0.72048718148788304</v>
+        <v>0.70962958705120605</v>
       </c>
       <c r="R21">
-        <v>33.136001490524201</v>
+        <v>29.151854502294501</v>
       </c>
       <c r="S21">
-        <v>894.10854918167104</v>
+        <v>881.86956981683795</v>
       </c>
       <c r="T21">
-        <v>0.71967732858031097</v>
+        <v>0.71010706370459398</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -30168,31 +30171,31 @@
         <v>0.71684324246126896</v>
       </c>
       <c r="L22">
-        <v>177.80563192530701</v>
+        <v>174.37340371282701</v>
       </c>
       <c r="M22">
-        <v>780.148474098169</v>
+        <v>785.74329669606698</v>
       </c>
       <c r="N22">
-        <v>0.70840355356234097</v>
+        <v>0.71554379249597699</v>
       </c>
       <c r="O22">
-        <v>177.72325560438401</v>
+        <v>174.471248039523</v>
       </c>
       <c r="P22">
-        <v>785.25018372940201</v>
+        <v>795.870169128322</v>
       </c>
       <c r="Q22">
-        <v>0.708333932537075</v>
+        <v>0.71667825372239002</v>
       </c>
       <c r="R22">
-        <v>177.640879283461</v>
+        <v>174.569092366219</v>
       </c>
       <c r="S22">
-        <v>790.35189336063604</v>
+        <v>805.99704156057601</v>
       </c>
       <c r="T22">
-        <v>0.70826431151180902</v>
+        <v>0.71781271494880206</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -30227,31 +30230,31 @@
         <v>0.70282487076144096</v>
       </c>
       <c r="L23">
-        <v>402.14431192913798</v>
+        <v>402.61320821931503</v>
       </c>
       <c r="M23">
-        <v>705.74621663434698</v>
+        <v>717.29267704757899</v>
       </c>
       <c r="N23">
-        <v>0.69179921623726404</v>
+        <v>0.69969052049724501</v>
       </c>
       <c r="O23">
-        <v>403.81123535391202</v>
+        <v>403.82204766932603</v>
       </c>
       <c r="P23">
-        <v>724.13115926147304</v>
+        <v>735.97384496628194</v>
       </c>
       <c r="Q23">
-        <v>0.69229806243879299</v>
+        <v>0.70109668414573101</v>
       </c>
       <c r="R23">
-        <v>405.47815877868601</v>
+        <v>405.03088711933702</v>
       </c>
       <c r="S23">
-        <v>742.51610188859695</v>
+        <v>754.65501288498604</v>
       </c>
       <c r="T23">
-        <v>0.69279690864032195</v>
+        <v>0.70250284779421601</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -30286,31 +30289,31 @@
         <v>0.67673963366346601</v>
       </c>
       <c r="L24">
-        <v>725.98379631410296</v>
+        <v>723.840633671467</v>
       </c>
       <c r="M24">
-        <v>671.94936825949605</v>
+        <v>678.08874513839805</v>
       </c>
       <c r="N24">
-        <v>0.67325227011894195</v>
+        <v>0.67332800944378501</v>
       </c>
       <c r="O24">
-        <v>729.85400705665802</v>
+        <v>725.371047897067</v>
       </c>
       <c r="P24">
-        <v>709.00768326535001</v>
+        <v>711.24552705841904</v>
       </c>
       <c r="Q24">
-        <v>0.67414781889175501</v>
+        <v>0.67471139301703398</v>
       </c>
       <c r="R24">
-        <v>733.72421779921206</v>
+        <v>726.901462122667</v>
       </c>
       <c r="S24">
-        <v>746.06599827120397</v>
+        <v>744.40230897844003</v>
       </c>
       <c r="T24">
-        <v>0.67504336766456696</v>
+        <v>0.67609477659028405</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -30345,31 +30348,31 @@
         <v>0.64921165895062904</v>
       </c>
       <c r="L25">
-        <v>1166.4004629032199</v>
+        <v>1155.96430182483</v>
       </c>
       <c r="M25">
-        <v>674.22275247926405</v>
+        <v>672.43753796802002</v>
       </c>
       <c r="N25">
-        <v>0.65453096290609203</v>
+        <v>0.64772178559601201</v>
       </c>
       <c r="O25">
-        <v>1172.9279485356401</v>
+        <v>1157.9362050827499</v>
       </c>
       <c r="P25">
-        <v>735.344579246683</v>
+        <v>729.34936148879501</v>
       </c>
       <c r="Q25">
-        <v>0.65565144959467603</v>
+        <v>0.64888723133800297</v>
       </c>
       <c r="R25">
-        <v>1179.45543416806</v>
+        <v>1159.90810834067</v>
       </c>
       <c r="S25">
-        <v>796.46640601410297</v>
+        <v>786.26118500956898</v>
       </c>
       <c r="T25">
-        <v>0.65677193628326003</v>
+        <v>0.65005267707999403</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -30404,31 +30407,31 @@
         <v>0.63044096392610305</v>
       </c>
       <c r="L26">
-        <v>1638.93411403871</v>
+        <v>1622.4493617687999</v>
       </c>
       <c r="M26">
-        <v>700.68960841254398</v>
+        <v>695.43945437145805</v>
       </c>
       <c r="N26">
-        <v>0.63996394031786397</v>
+        <v>0.63293325637311704</v>
       </c>
       <c r="O26">
-        <v>1648.04455217432</v>
+        <v>1625.32190847437</v>
       </c>
       <c r="P26">
-        <v>786.19028477473603</v>
+        <v>779.94481340254094</v>
       </c>
       <c r="Q26">
-        <v>0.64114063512991704</v>
+        <v>0.63384346815953496</v>
       </c>
       <c r="R26">
-        <v>1657.1549903099401</v>
+        <v>1628.1944551799299</v>
       </c>
       <c r="S26">
-        <v>871.69096113692694</v>
+        <v>864.45017243362599</v>
       </c>
       <c r="T26">
-        <v>0.64231732994197099</v>
+        <v>0.634753679945953</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -30463,31 +30466,31 @@
         <v>0.63062858235165098</v>
       </c>
       <c r="L27">
-        <v>1740.4706895195</v>
+        <v>1723.3413143221901</v>
       </c>
       <c r="M27">
-        <v>708.03119279929604</v>
+        <v>702.68335255373495</v>
       </c>
       <c r="N27">
-        <v>0.63740354229742902</v>
+        <v>0.63105598561667398</v>
       </c>
       <c r="O27">
-        <v>1750.1094376138601</v>
+        <v>1726.45912987207</v>
       </c>
       <c r="P27">
-        <v>798.60667071111902</v>
+        <v>793.156312641005</v>
       </c>
       <c r="Q27">
-        <v>0.63857720224627401</v>
+        <v>0.63191618560031304</v>
       </c>
       <c r="R27">
-        <v>1759.74818570823</v>
+        <v>1729.5769454219401</v>
       </c>
       <c r="S27">
-        <v>889.18214862294099</v>
+        <v>883.62927272827505</v>
       </c>
       <c r="T27">
-        <v>0.63975086219511901</v>
+        <v>0.632776385583951</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -30522,31 +30525,31 @@
         <v>0.63051477993698701</v>
       </c>
       <c r="L28" s="9">
-        <v>2465.27085398596</v>
+        <v>2449.2130137742602</v>
       </c>
       <c r="M28" s="8">
-        <v>768.83951272524098</v>
+        <v>767.12069253163702</v>
       </c>
       <c r="N28" s="8">
-        <v>0.623638255991671</v>
+        <v>0.62582215575492595</v>
       </c>
       <c r="O28" s="4">
-        <v>2478.4748521143501</v>
+        <v>2454.44084827712</v>
       </c>
       <c r="P28">
-        <v>894.25878116430397</v>
+        <v>898.65610979919302</v>
       </c>
       <c r="Q28">
-        <v>0.62469332454526605</v>
+        <v>0.62640617696969203</v>
       </c>
       <c r="R28">
-        <v>2491.6788502427498</v>
+        <v>2459.6686827799799</v>
       </c>
       <c r="S28">
-        <v>1019.67804960337</v>
+        <v>1030.19152706675</v>
       </c>
       <c r="T28">
-        <v>0.62574839309885999</v>
+        <v>0.626990198184457</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -30581,31 +30584,31 @@
         <v>0.62759345367496</v>
       </c>
       <c r="L29">
-        <v>3357.8773341256101</v>
+        <v>3348.1407448404202</v>
       </c>
       <c r="M29">
-        <v>852.11253576274805</v>
+        <v>857.90621475764499</v>
       </c>
       <c r="N29">
-        <v>0.61500335168753495</v>
+        <v>0.62620805103041</v>
       </c>
       <c r="O29">
-        <v>3375.1005698601198</v>
+        <v>3356.3775627571299</v>
       </c>
       <c r="P29">
-        <v>1017.76573411189</v>
+        <v>1032.8691937490601</v>
       </c>
       <c r="Q29">
-        <v>0.615768064190367</v>
+        <v>0.62666986046999695</v>
       </c>
       <c r="R29">
-        <v>3392.3238055946299</v>
+        <v>3364.6143806738301</v>
       </c>
       <c r="S29">
-        <v>1183.41893246103</v>
+        <v>1207.83217274048</v>
       </c>
       <c r="T29">
-        <v>0.61653277669319995</v>
+        <v>0.62713166990958402</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -30640,31 +30643,31 @@
         <v>0.62490475482778896</v>
       </c>
       <c r="L30">
-        <v>3818.8468480930501</v>
+        <v>3809.4556894782399</v>
       </c>
       <c r="M30">
-        <v>895.70616443255801</v>
+        <v>903.42848469036505</v>
       </c>
       <c r="N30">
-        <v>0.61326255937492902</v>
+        <v>0.624224255061815</v>
       </c>
       <c r="O30">
-        <v>3838.0268541957098</v>
+        <v>3819.2478350770298</v>
       </c>
       <c r="P30">
-        <v>1081.2231642148799</v>
+        <v>1096.6863293025999</v>
       </c>
       <c r="Q30">
-        <v>0.61384057343605802</v>
+        <v>0.62471653806425997</v>
       </c>
       <c r="R30">
-        <v>3857.20686029836</v>
+        <v>3829.0399806758201</v>
       </c>
       <c r="S30">
-        <v>1266.7401639972099</v>
+        <v>1289.9441739148399</v>
       </c>
       <c r="T30">
-        <v>0.61441858749718803</v>
+        <v>0.62520882106670395</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -30699,31 +30702,31 @@
         <v>0.61257763782007302</v>
       </c>
       <c r="L31">
-        <v>4435.3665077614696</v>
+        <v>4418.4416153094398</v>
       </c>
       <c r="M31">
-        <v>953.31508541746098</v>
+        <v>958.97067590851998</v>
       </c>
       <c r="N31">
-        <v>0.61326707708373596</v>
+        <v>0.61548643441733097</v>
       </c>
       <c r="O31">
-        <v>4457.0629686741804</v>
+        <v>4430.1964132991498</v>
       </c>
       <c r="P31">
-        <v>1164.5923530595101</v>
+        <v>1171.7586633789001</v>
       </c>
       <c r="Q31">
-        <v>0.61356966888029596</v>
+        <v>0.61611342416729298</v>
       </c>
       <c r="R31">
-        <v>4478.7594295868903</v>
+        <v>4441.9512112888697</v>
       </c>
       <c r="S31">
-        <v>1375.8696207015701</v>
+        <v>1384.54665084928</v>
       </c>
       <c r="T31">
-        <v>0.61387226067685496</v>
+        <v>0.61674041391725698</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -30758,31 +30761,31 @@
         <v>0.60375951511530901</v>
       </c>
       <c r="L32">
-        <v>4921.9544400271097</v>
+        <v>4889.8091686149701</v>
       </c>
       <c r="M32">
-        <v>997.80049319743</v>
+        <v>996.75898384619995</v>
       </c>
       <c r="N32">
-        <v>0.61490027104282396</v>
+        <v>0.60182505694496402</v>
       </c>
       <c r="O32">
-        <v>4945.5673075312798</v>
+        <v>4902.9644781163397</v>
       </c>
       <c r="P32">
-        <v>1228.83662758384</v>
+        <v>1220.78439795182</v>
       </c>
       <c r="Q32">
-        <v>0.61496992045333099</v>
+        <v>0.60263009900029496</v>
       </c>
       <c r="R32">
-        <v>4969.1801750354498</v>
+        <v>4916.1197876177102</v>
       </c>
       <c r="S32">
-        <v>1459.8727619702599</v>
+        <v>1444.80981205744</v>
       </c>
       <c r="T32">
-        <v>0.61503956986383801</v>
+        <v>0.60343514105562801</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -30929,31 +30932,31 @@
         <v>49</v>
       </c>
       <c r="L36">
-        <v>-476.08648315516501</v>
+        <v>2070.4537616252401</v>
       </c>
       <c r="M36">
-        <v>1405.12342529731</v>
+        <v>1602.6807665399499</v>
       </c>
       <c r="N36">
-        <v>0.43205924345292301</v>
+        <v>0.300701972016923</v>
       </c>
       <c r="O36">
-        <v>-453.345939279091</v>
+        <v>1952.5609916503299</v>
       </c>
       <c r="P36">
-        <v>1352.8663773933699</v>
+        <v>1303.4575890057699</v>
       </c>
       <c r="Q36">
-        <v>0.436739360800667</v>
+        <v>0.29042986770016799</v>
       </c>
       <c r="R36">
-        <v>-430.60539540301801</v>
+        <v>1834.66822167542</v>
       </c>
       <c r="S36">
-        <v>1300.6093294894299</v>
+        <v>1004.2344114716</v>
       </c>
       <c r="T36">
-        <v>0.44141947814841198</v>
+        <v>0.28015776338341403</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -30988,31 +30991,31 @@
         <v>49</v>
       </c>
       <c r="L37">
-        <v>-130.699137866782</v>
+        <v>769.28402594417196</v>
       </c>
       <c r="M37">
-        <v>1093.27173189626</v>
+        <v>1097.8946495898399</v>
       </c>
       <c r="N37">
-        <v>0.44736278283321201</v>
+        <v>0.397727773148432</v>
       </c>
       <c r="O37">
-        <v>-116.845891565603</v>
+        <v>718.25247370795705</v>
       </c>
       <c r="P37">
-        <v>1059.85488860652</v>
+        <v>980.80252213328004</v>
       </c>
       <c r="Q37">
-        <v>0.450345863430826</v>
+        <v>0.39335619103916297</v>
       </c>
       <c r="R37">
-        <v>-102.992645264423</v>
+        <v>667.22092147174897</v>
       </c>
       <c r="S37">
-        <v>1026.4380453167701</v>
+        <v>863.71039467672301</v>
       </c>
       <c r="T37">
-        <v>0.45332894402843998</v>
+        <v>0.388984608929895</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
@@ -31047,31 +31050,31 @@
         <v>49</v>
       </c>
       <c r="L38">
-        <v>198.298723866476</v>
+        <v>412.20625168948698</v>
       </c>
       <c r="M38">
-        <v>884.21863429833502</v>
+        <v>856.29197145364799</v>
       </c>
       <c r="N38">
-        <v>0.45844392565599201</v>
+        <v>0.44569353073927598</v>
       </c>
       <c r="O38">
-        <v>205.82896053641201</v>
+        <v>396.013677451109</v>
       </c>
       <c r="P38">
-        <v>872.92811526840899</v>
+        <v>831.18054756257197</v>
       </c>
       <c r="Q38">
-        <v>0.46007065547840698</v>
+        <v>0.44433260326983798</v>
       </c>
       <c r="R38">
-        <v>213.359197206348</v>
+        <v>379.82110321273598</v>
       </c>
       <c r="S38">
-        <v>861.63759623848296</v>
+        <v>806.06912367149698</v>
       </c>
       <c r="T38">
-        <v>0.46169738530082299</v>
+        <v>0.44297167580039998</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -31106,31 +31109,31 @@
         <v>0.46545597145648399</v>
       </c>
       <c r="L39">
-        <v>542.97273045320605</v>
+        <v>547.74428273313004</v>
       </c>
       <c r="M39">
-        <v>762.53360427435803</v>
+        <v>753.20727953816004</v>
       </c>
       <c r="N39">
-        <v>0.46580861379627098</v>
+        <v>0.46543611916955102</v>
       </c>
       <c r="O39">
-        <v>546.74424543555006</v>
+        <v>545.88593828318199</v>
       </c>
       <c r="P39">
-        <v>776.655529149882</v>
+        <v>771.56877272717998</v>
       </c>
       <c r="Q39">
-        <v>0.466419678818419</v>
+        <v>0.46523511063273199</v>
       </c>
       <c r="R39">
-        <v>550.51576041789303</v>
+        <v>544.02759383323598</v>
       </c>
       <c r="S39">
-        <v>790.77745402540495</v>
+        <v>789.93026591620003</v>
       </c>
       <c r="T39">
-        <v>0.46703074384056797</v>
+        <v>0.465034102095914</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -31165,31 +31168,31 @@
         <v>49</v>
       </c>
       <c r="L40">
-        <v>935.38851030200703</v>
+        <v>915.41586116505198</v>
       </c>
       <c r="M40">
-        <v>712.78611359517004</v>
+        <v>719.76948328114395</v>
       </c>
       <c r="N40">
-        <v>0.46996278912905798</v>
+        <v>0.471107339540415</v>
       </c>
       <c r="O40">
-        <v>937.96559154040801</v>
+        <v>916.76464920874798</v>
       </c>
       <c r="P40">
-        <v>755.60660202176996</v>
+        <v>763.72109877178605</v>
       </c>
       <c r="Q40">
-        <v>0.46989887532587099</v>
+        <v>0.47106170275575399</v>
       </c>
       <c r="R40">
-        <v>940.54267277881002</v>
+        <v>918.11343725246104</v>
       </c>
       <c r="S40">
-        <v>798.42709044836897</v>
+        <v>807.67271426243099</v>
       </c>
       <c r="T40">
-        <v>0.469834961522684</v>
+        <v>0.47101606597109302</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -31224,31 +31227,31 @@
         <v>0.47381962392822202</v>
       </c>
       <c r="L41">
-        <v>1325.3713084456001</v>
+        <v>1315.9694171757501</v>
       </c>
       <c r="M41">
-        <v>715.30282426629799</v>
+        <v>723.02584877542495</v>
       </c>
       <c r="N41">
-        <v>0.47134135109165498</v>
+        <v>0.47141842532749301</v>
       </c>
       <c r="O41">
-        <v>1328.92674706194</v>
+        <v>1316.7708608599301</v>
       </c>
       <c r="P41">
-        <v>784.76961933794405</v>
+        <v>789.32023149388999</v>
       </c>
       <c r="Q41">
-        <v>0.47097373719661401</v>
+        <v>0.47121053665513002</v>
       </c>
       <c r="R41">
-        <v>1332.4821856782901</v>
+        <v>1317.57230454413</v>
       </c>
       <c r="S41">
-        <v>854.23641440958795</v>
+        <v>855.61461421236004</v>
       </c>
       <c r="T41">
-        <v>0.47060612330157298</v>
+        <v>0.47100264798276797</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -31283,31 +31286,31 @@
         <v>0.47261625558908898</v>
       </c>
       <c r="L42">
-        <v>1407.61169182147</v>
+        <v>1399.75506398316</v>
       </c>
       <c r="M42">
-        <v>719.545634031605</v>
+        <v>726.31053133697196</v>
       </c>
       <c r="N42">
-        <v>0.47141239352936098</v>
+        <v>0.47129689042422201</v>
       </c>
       <c r="O42">
-        <v>1411.5586272595799</v>
+        <v>1400.4216975235299</v>
       </c>
       <c r="P42">
-        <v>794.35080565490898</v>
+        <v>797.57689773783</v>
       </c>
       <c r="Q42">
-        <v>0.47101418687577101</v>
+        <v>0.471055323404309</v>
       </c>
       <c r="R42">
-        <v>1415.50556269769</v>
+        <v>1401.0883310639199</v>
       </c>
       <c r="S42">
-        <v>869.15597727821205</v>
+        <v>868.84326413867598</v>
       </c>
       <c r="T42">
-        <v>0.47061598022217999</v>
+        <v>0.47081375638439599</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -31342,31 +31345,31 @@
         <v>0.47018648409519898</v>
       </c>
       <c r="L43">
-        <v>1991.7079034202</v>
+        <v>1984.33473978302</v>
       </c>
       <c r="M43">
-        <v>767.381637354497</v>
+        <v>765.77408876231505</v>
       </c>
       <c r="N43">
-        <v>0.47066336887219001</v>
+        <v>0.47015533861462899</v>
       </c>
       <c r="O43">
-        <v>1999.5889810016699</v>
+        <v>1985.5279015040101</v>
       </c>
       <c r="P43">
-        <v>877.45761182013405</v>
+        <v>874.66968974920201</v>
       </c>
       <c r="Q43">
-        <v>0.47027155534312798</v>
+        <v>0.469826841231412</v>
       </c>
       <c r="R43">
-        <v>2007.4700585831399</v>
+        <v>1986.7210632250101</v>
       </c>
       <c r="S43">
-        <v>987.53358628576996</v>
+        <v>983.56529073606498</v>
       </c>
       <c r="T43">
-        <v>0.469879741814066</v>
+        <v>0.469498343848194</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -31401,31 +31404,31 @@
         <v>0.46748399310015898</v>
       </c>
       <c r="L44">
-        <v>2719.7427735067999</v>
+        <v>2705.7889454477099</v>
       </c>
       <c r="M44">
-        <v>840.86359533468396</v>
+        <v>837.12421420181101</v>
       </c>
       <c r="N44">
-        <v>0.46822165703255397</v>
+        <v>0.46851708987673102</v>
       </c>
       <c r="O44">
-        <v>2734.12228117528</v>
+        <v>2711.6754470974101</v>
       </c>
       <c r="P44">
-        <v>989.49649228828002</v>
+        <v>991.53582019791395</v>
       </c>
       <c r="Q44">
-        <v>0.46817692260295102</v>
+        <v>0.46847802052781901</v>
       </c>
       <c r="R44">
-        <v>2748.5017888437601</v>
+        <v>2717.5619487471099</v>
       </c>
       <c r="S44">
-        <v>1138.1293892418801</v>
+        <v>1145.9474261939999</v>
       </c>
       <c r="T44">
-        <v>0.46813218817334901</v>
+        <v>0.46843895117890799</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -31460,31 +31463,31 @@
         <v>0.47059621256220302</v>
       </c>
       <c r="L45">
-        <v>3102.8619382465399</v>
+        <v>3087.64941081298</v>
       </c>
       <c r="M45">
-        <v>878.18619776765104</v>
+        <v>877.34892526303304</v>
       </c>
       <c r="N45">
-        <v>0.46670544939976</v>
+        <v>0.467307760547436</v>
       </c>
       <c r="O45">
-        <v>3121.00233839579</v>
+        <v>3097.3037538869398</v>
       </c>
       <c r="P45">
-        <v>1045.24180637521</v>
+        <v>1051.63709549177</v>
       </c>
       <c r="Q45">
-        <v>0.46692804936423699</v>
+        <v>0.46754861624806898</v>
       </c>
       <c r="R45">
-        <v>3139.1427385450402</v>
+        <v>3106.9580969608801</v>
       </c>
       <c r="S45">
-        <v>1212.2974149827801</v>
+        <v>1225.92526572051</v>
       </c>
       <c r="T45">
-        <v>0.46715064932871297</v>
+        <v>0.46778947194870102</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
@@ -31519,31 +31522,31 @@
         <v>0.46551811113974301</v>
       </c>
       <c r="L46">
-        <v>3623.7819304898499</v>
+        <v>3607.8353828376798</v>
       </c>
       <c r="M46">
-        <v>924.56097974299701</v>
+        <v>928.75403707374596</v>
       </c>
       <c r="N46">
-        <v>0.46459319988546</v>
+        <v>0.46502335969716502</v>
       </c>
       <c r="O46">
-        <v>3647.22415618899</v>
+        <v>3623.4003246114298</v>
       </c>
       <c r="P46">
-        <v>1115.03691883018</v>
+        <v>1123.12313692978</v>
       </c>
       <c r="Q46">
-        <v>0.46523623053024998</v>
+        <v>0.465724491972133</v>
       </c>
       <c r="R46">
-        <v>3670.6663818881302</v>
+        <v>3638.9652663851698</v>
       </c>
       <c r="S46">
-        <v>1305.51285791736</v>
+        <v>1317.4922367858101</v>
       </c>
       <c r="T46">
-        <v>0.46587926117503897</v>
+        <v>0.46642562424710099</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -31578,31 +31581,31 @@
         <v>0.467259213215446</v>
       </c>
       <c r="L47">
-        <v>4041.8614943776001</v>
+        <v>4022.65764120943</v>
       </c>
       <c r="M47">
-        <v>957.44381458286705</v>
+        <v>963.691728248392</v>
       </c>
       <c r="N47">
-        <v>0.46292285932053701</v>
+        <v>0.46257253765678902</v>
       </c>
       <c r="O47">
-        <v>4069.6468079132301</v>
+        <v>4043.2656580462499</v>
       </c>
       <c r="P47">
-        <v>1165.5770840242601</v>
+        <v>1167.37795444631</v>
       </c>
       <c r="Q47">
-        <v>0.46393638806806398</v>
+        <v>0.46367589977865298</v>
       </c>
       <c r="R47">
-        <v>4097.43212144886</v>
+        <v>4063.8736748830902</v>
       </c>
       <c r="S47">
-        <v>1373.7103534656501</v>
+        <v>1371.0641806441699</v>
       </c>
       <c r="T47">
-        <v>0.464949916815591</v>
+        <v>0.46477926190051699</v>
       </c>
     </row>
   </sheetData>
@@ -31643,8 +31646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
   <dimension ref="B3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I35" sqref="B32:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -31686,7 +31689,7 @@
       </c>
       <c r="D5">
         <f>C12/1000</f>
-        <v>1.7217824084012501</v>
+        <v>1.8010977482444401</v>
       </c>
       <c r="E5">
         <v>1.8009999999999999</v>
@@ -31705,7 +31708,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.97695631979742092</v>
+        <v>1.0131010128053801</v>
       </c>
       <c r="E6">
         <v>0.622</v>
@@ -31724,7 +31727,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.89646959680438709</v>
+        <v>0.85670654653141298</v>
       </c>
       <c r="E7">
         <v>0.51800000000000002</v>
@@ -31743,7 +31746,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.87764282711932595</v>
+        <v>0.81876682645388499</v>
       </c>
       <c r="E8">
         <v>0.505</v>
@@ -31762,7 +31765,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.98701070888513698</v>
+        <v>0.80387616088661606</v>
       </c>
       <c r="E9">
         <v>0.505</v>
@@ -31781,7 +31784,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.4598618610075222</v>
+        <v>5.2935482949217336</v>
       </c>
       <c r="E10">
         <v>3.9119999999999999</v>
@@ -31795,7 +31798,7 @@
         <v>1855.61590285229</v>
       </c>
       <c r="C12">
-        <v>1721.78240840125</v>
+        <v>1801.09774824444</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -31803,7 +31806,7 @@
         <v>917.74235268904101</v>
       </c>
       <c r="C13">
-        <v>976.95631979742097</v>
+        <v>1013.10101280538</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -31811,7 +31814,7 @@
         <v>714.70070088930504</v>
       </c>
       <c r="C14">
-        <v>896.46959680438704</v>
+        <v>856.70654653141298</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -31819,7 +31822,7 @@
         <v>656.45493639253402</v>
       </c>
       <c r="C15">
-        <v>877.64282711932594</v>
+        <v>818.76682645388496</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -31827,7 +31830,7 @@
         <v>638.07968558066602</v>
       </c>
       <c r="C16">
-        <v>987.01070888513698</v>
+        <v>803.87616088661605</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -31837,7 +31840,7 @@
       </c>
       <c r="C17">
         <f>SUM(C12:C16)</f>
-        <v>5459.8618610075218</v>
+        <v>5293.5482949217339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAde scripts to run FASTnAT for model verification, and for correspoding plots.
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7872000-F6B4-4066-8A57-C5717E7C796F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194C801-2DDA-467B-B4E7-8867DAEDC282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="5" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
   <sheets>
     <sheet name="randomCalculations" sheetId="2" r:id="rId1"/>
@@ -7822,7 +7822,7 @@
           <c:spPr>
             <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7837,7 +7837,7 @@
               </a:solidFill>
               <a:ln w="44450">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -7993,7 +7993,7 @@
           <c:spPr>
             <a:ln w="38100" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -8009,7 +8009,7 @@
               </a:solidFill>
               <a:ln w="44450">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -8420,7 +8420,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>FASTnAT optimised</c:v>
+            <c:v>FASTnAT baseline</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -8495,11 +8495,11 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>FLORIS</c:v>
+            <c:v>FLORIS baseline</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -8534,7 +8534,7 @@
           <c:spPr>
             <a:pattFill prst="wdUpDiag">
               <a:fgClr>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FF0000"/>
               </a:fgClr>
               <a:bgClr>
                 <a:schemeClr val="bg1"/>
@@ -29118,7 +29118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F248FD9-301D-457F-AE14-7A8D9661D287}">
   <dimension ref="A2:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <selection activeCell="R36" sqref="R36:T47"/>
     </sheetView>
   </sheetViews>
@@ -31610,16 +31610,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="L18:T18"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="R19:T19"/>
     <mergeCell ref="L2:T2"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="B33:J33"/>
@@ -31636,6 +31626,16 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="L33:T33"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="L18:T18"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31646,8 +31646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
   <dimension ref="B3:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="B32:I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made changes to wake model, it now considers near wake and turbines not operating for wind speed lower than cut-in speed
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F194C801-2DDA-467B-B4E7-8867DAEDC282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9EAB39-2BE1-4E20-914A-BD8F9D156D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="65">
   <si>
     <t>baseline control</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Gebraad: FLORIS</t>
+  </si>
+  <si>
+    <t>Gebraad: SOWFA</t>
+  </si>
+  <si>
+    <t>Wind speed</t>
+  </si>
+  <si>
+    <t>turbulence intensity</t>
   </si>
 </sst>
 </file>
@@ -7729,13 +7738,183 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>FLORIS baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="28575">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.8009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.622</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SOWFA baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="28575">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$G$5:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.8939999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76400000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F0D-4B56-A0A0-4A8A664C6472}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>FASTnAT baseline</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -7750,7 +7929,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="44450">
+              <a:ln w="28575">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -7814,16 +7993,17 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>FLORIS baseline</c:v>
+            <c:v>FLORIS optimised</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -7833,9 +8013,9 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:ln w="44450">
+              <a:ln w="28575">
                 <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
@@ -7869,24 +8049,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>compOptGebradd!$E$5:$E$9</c:f>
+              <c:f>compOptGebradd!$F$5:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.8009999999999999</c:v>
+                  <c:v>1.5669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.622</c:v>
+                  <c:v>0.72499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51800000000000002</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.505</c:v>
+                  <c:v>0.82899999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.505</c:v>
+                  <c:v>0.97199999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7894,18 +8074,105 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
+              <c16:uniqueId val="{00000003-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>SOWFA optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="28575">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$H$5:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3F0D-4B56-A0A0-4A8A664C6472}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="5"/>
           <c:tx>
             <c:v>FASTnAT optimised</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -7919,9 +8186,9 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="44450">
+              <a:ln w="28575">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -7960,19 +8227,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.8010977482444401</c:v>
+                  <c:v>1.73078111002158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0131010128053801</c:v>
+                  <c:v>0.98085151380082203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85670654653141298</c:v>
+                  <c:v>0.89335176153722495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.81876682645388499</c:v>
+                  <c:v>0.91024035557522909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80387616088661606</c:v>
+                  <c:v>0.93967051520564493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7981,92 +8248,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>FASTnAT optimised</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="44450">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$B$5:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$F$5:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.5669999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.79</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.82899999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.97199999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-EDCB-4D26-8B03-0E6D9BEF4ED1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8434,6 +8615,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>compOptGebradd!$C$10</c:f>
@@ -8473,6 +8663,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>compOptGebradd!$D$10</c:f>
@@ -8480,7 +8679,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.2935482949217336</c:v>
+                  <c:v>5.4548952561405004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8507,6 +8706,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>compOptGebradd!$E$10</c:f>
@@ -8546,6 +8754,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>compOptGebradd!$F$10</c:f>
@@ -8561,6 +8778,116 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-00E2-467B-B1EB-CF8E37BC7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>SOWFA baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-0DD2-45B7-9AD3-16A87FFBDFAA}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.5510000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DD2-45B7-9AD3-16A87FFBDFAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>SOWFA optimised</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="92D050"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>compOptGebradd!$C$19:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compOptGebradd!$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4.1029999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0DD2-45B7-9AD3-16A87FFBDFAA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8584,6 +8911,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8748,8 +9076,1077 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>pitch</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$I$5:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.39882543714213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3582069880760201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3958175904724599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8447543320842001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96390453372662499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-991D-4DCF-97C6-9073E687DE07}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="521064656"/>
+        <c:axId val="521062416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="521064656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Turbine number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521062416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="521062416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>β</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>o</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521064656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15587206366935857"/>
+          <c:y val="3.5795251072238771E-2"/>
+          <c:w val="0.81794841592898326"/>
+          <c:h val="0.61305430144162132"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Turbine 1 - Literature</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.077</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0359999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.5220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2710000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8150000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3140000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-414E-4232-A2AA-5E623D6CF4FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Turbine 1 - FASTnAT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$B$23:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$C$23:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.6925703267444696</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6931287332950404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6935400844400297</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6937982802861802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.6938101622498003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-414E-4232-A2AA-5E623D6CF4FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Turbine 2 - Literature</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0540000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0590000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.9870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0780000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.359</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-414E-4232-A2AA-5E623D6CF4FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Turbine 2 - FASTnAT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$D$23:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>getGebraad2.6!$E$23:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.5062845798801501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3960506045132597</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2945061122059105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2025484157053192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1116668207164295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-414E-4232-A2AA-5E623D6CF4FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="556640568"/>
+        <c:axId val="556643128"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="556640568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>Pitch</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
+                  <a:t> offset [deg]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556643128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="556643128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9.5"/>
+          <c:min val="6.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:t>TSR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556640568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.1554345279286843E-2"/>
+          <c:y val="0.78487218762795707"/>
+          <c:w val="0.96381149841162606"/>
+          <c:h val="0.20079241870411504"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
@@ -8775,7 +10172,523 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>baseline case</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$P$4:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3633893020423198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8882762932856396</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7375244634637204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.68834067938222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EAA8-49EA-8E78-20510F16E023}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>optimised case</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>compOptGebradd!$Q$4:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7580800347977501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5614172705416101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5117378544789304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4127158655455796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EAA8-49EA-8E78-20510F16E023}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="521064656"/>
+        <c:axId val="521062416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="521064656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Turbine number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521062416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="521062416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>β</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>o</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1200">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521064656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9497,648 +11410,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.15587206366935857"/>
-          <c:y val="3.5795251072238771E-2"/>
-          <c:w val="0.81794841592898326"/>
-          <c:h val="0.61305430144162132"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Turbine 1 - Literature</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$B$5:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-2.3E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0270000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.077</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0359999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$C$5:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>8.5220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.43</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.2710000000000008</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.8150000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.3140000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-414E-4232-A2AA-5E623D6CF4FE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Turbine 1 - FASTnAT</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$B$23:$B$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$C$23:$C$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>7.6925703267444696</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.6931287332950404</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.6935400844400297</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.6937982802861802</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.6938101622498003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-414E-4232-A2AA-5E623D6CF4FE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Turbine 2 - Literature</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$D$5:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2.3E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.036</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0270000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0540000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0590000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$E$5:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6.9870000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.0179999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0780000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.359</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-414E-4232-A2AA-5E623D6CF4FE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Turbine 2 - FASTnAT</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$D$23:$D$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>getGebraad2.6!$E$23:$E$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>8.5062845798801501</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.3960506045132597</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.2945061122059105</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.2025484157053192</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.1116668207164295</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-414E-4232-A2AA-5E623D6CF4FE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="556640568"/>
-        <c:axId val="556643128"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="556640568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="4"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1600"/>
-                  <a:t>Pitch</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
-                  <a:t> offset [deg]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="1600"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="556643128"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="556643128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="9.5"/>
-          <c:min val="6.5"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1600"/>
-                  <a:t>TSR</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="556640568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="2.1554345279286843E-2"/>
-          <c:y val="0.78487218762795707"/>
-          <c:w val="0.96381149841162606"/>
-          <c:h val="0.20079241870411504"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -12977,6 +14248,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -15768,6 +17053,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors21.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -21712,6 +23077,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -26451,16 +28848,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>128184</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>51275</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>205095</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>119642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>606751</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>170916</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>205099</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>119641</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26487,16 +28884,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>8546</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>17093</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>8544</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>128187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>136732</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>136734</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>25637</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>119642</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26516,6 +28913,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>119642</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>102549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>119645</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>68365</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64DCCBAF-0FD1-4BFE-BAEE-B6F8490B667B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>34183</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>153824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>34187</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>119640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884EACAC-D669-462D-8446-5954E9DDBAAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -28885,7 +31358,7 @@
   <dimension ref="C2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -31610,6 +34083,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="O34:Q34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="L18:T18"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
     <mergeCell ref="L2:T2"/>
     <mergeCell ref="L3:T3"/>
     <mergeCell ref="B33:J33"/>
@@ -31626,16 +34109,6 @@
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="H19:J19"/>
     <mergeCell ref="L33:T33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="O34:Q34"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="L18:T18"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="R19:T19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31644,15 +34117,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
-  <dimension ref="B3:F17"/>
+  <dimension ref="B2:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="13"/>
+      <c r="S2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="13"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
@@ -31661,8 +34144,24 @@
         <v>61</v>
       </c>
       <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>55</v>
       </c>
@@ -31678,8 +34177,29 @@
       <c r="F4" t="s">
         <v>58</v>
       </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <v>6</v>
+      </c>
+      <c r="T4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -31689,7 +34209,7 @@
       </c>
       <c r="D5">
         <f>C12/1000</f>
-        <v>1.8010977482444401</v>
+        <v>1.73078111002158</v>
       </c>
       <c r="E5">
         <v>1.8009999999999999</v>
@@ -31697,8 +34217,29 @@
       <c r="F5">
         <v>1.5669999999999999</v>
       </c>
+      <c r="G5">
+        <v>1.8939999999999999</v>
+      </c>
+      <c r="H5">
+        <v>1.728</v>
+      </c>
+      <c r="I5">
+        <v>2.39882543714213</v>
+      </c>
+      <c r="P5">
+        <v>6.3633893020423198</v>
+      </c>
+      <c r="Q5">
+        <v>6.7580800347977501</v>
+      </c>
+      <c r="S5">
+        <v>14.359720744636</v>
+      </c>
+      <c r="T5">
+        <v>11.9791683297394</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
@@ -31708,7 +34249,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.0131010128053801</v>
+        <v>0.98085151380082203</v>
       </c>
       <c r="E6">
         <v>0.622</v>
@@ -31716,8 +34257,29 @@
       <c r="F6">
         <v>0.72499999999999998</v>
       </c>
+      <c r="G6">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="H6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="I6">
+        <v>3.3582069880760201</v>
+      </c>
+      <c r="P6">
+        <v>5.8882762932856396</v>
+      </c>
+      <c r="Q6">
+        <v>6.5614172705416101</v>
+      </c>
+      <c r="S6">
+        <v>15.650566973618799</v>
+      </c>
+      <c r="T6">
+        <v>11.299518394491001</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -31727,7 +34289,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.85670654653141298</v>
+        <v>0.89335176153722495</v>
       </c>
       <c r="E7">
         <v>0.51800000000000002</v>
@@ -31735,8 +34297,29 @@
       <c r="F7">
         <v>0.79</v>
       </c>
+      <c r="G7">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="H7">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="I7">
+        <v>3.3958175904724599</v>
+      </c>
+      <c r="P7">
+        <v>5.7375244634637204</v>
+      </c>
+      <c r="Q7">
+        <v>6.5117378544789304</v>
+      </c>
+      <c r="S7">
+        <v>16.262354187252601</v>
+      </c>
+      <c r="T7">
+        <v>11.3039257372472</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -31746,7 +34329,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.81876682645388499</v>
+        <v>0.91024035557522909</v>
       </c>
       <c r="E8">
         <v>0.505</v>
@@ -31754,8 +34337,29 @@
       <c r="F8">
         <v>0.82899999999999996</v>
       </c>
+      <c r="G8">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="H8">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="I8">
+        <v>2.8447543320842001</v>
+      </c>
+      <c r="P8">
+        <v>5.68834067938222</v>
+      </c>
+      <c r="Q8">
+        <v>6.4127158655455796</v>
+      </c>
+      <c r="S8">
+        <v>16.488511607784499</v>
+      </c>
+      <c r="T8">
+        <v>11.942586520688501</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -31765,7 +34369,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.80387616088661606</v>
+        <v>0.93967051520564493</v>
       </c>
       <c r="E9">
         <v>0.505</v>
@@ -31773,8 +34377,17 @@
       <c r="F9">
         <v>0.97199999999999998</v>
       </c>
+      <c r="G9">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.96390453372662499</v>
+      </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -31784,7 +34397,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.2935482949217336</v>
+        <v>5.4548952561405004</v>
       </c>
       <c r="E10">
         <v>3.9119999999999999</v>
@@ -31792,45 +34405,51 @@
       <c r="F10">
         <v>4.883</v>
       </c>
+      <c r="G10">
+        <v>4.5510000000000002</v>
+      </c>
+      <c r="H10">
+        <v>4.1029999999999998</v>
+      </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1855.61590285229</v>
       </c>
       <c r="C12">
-        <v>1801.09774824444</v>
+        <v>1730.7811100215799</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>917.74235268904101</v>
       </c>
       <c r="C13">
-        <v>1013.10101280538</v>
+        <v>980.85151380082198</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>714.70070088930504</v>
       </c>
       <c r="C14">
-        <v>856.70654653141298</v>
+        <v>893.351761537225</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>656.45493639253402</v>
       </c>
       <c r="C15">
-        <v>818.76682645388496</v>
+        <v>910.24035557522905</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>638.07968558066602</v>
       </c>
       <c r="C16">
-        <v>803.87616088661605</v>
+        <v>939.67051520564496</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -31840,13 +34459,16 @@
       </c>
       <c r="C17">
         <f>SUM(C12:C16)</f>
-        <v>5293.5482949217339</v>
+        <v>5454.8952561405004</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Made changes to FASTnAT functions due to verification conclusions.
</commit_message>
<xml_diff>
--- a/helpfulSheet.xlsx
+++ b/helpfulSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfram\Documents\GitHub\wind-farm-control-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9EAB39-2BE1-4E20-914A-BD8F9D156D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF00B44-B0F5-4559-B8DE-94D7506AB291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="26055" windowHeight="14158" firstSheet="1" activeTab="6" xr2:uid="{7A5FF4EF-FFAC-4D58-AB26-73838BBBD728}"/>
   </bookViews>
@@ -8292,9 +8292,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8302,9 +8302,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1100">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Turbine number</a:t>
@@ -8325,9 +8325,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -8344,12 +8344,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -8360,9 +8357,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -8405,9 +8402,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8415,24 +8412,24 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> Power</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                  <a:rPr lang="en-GB" sz="1400" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> [MW]</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1200">
+                <a:endParaRPr lang="en-GB" sz="1400">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                 </a:endParaRPr>
               </a:p>
@@ -8451,9 +8448,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -8470,12 +8467,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -8486,7 +8480,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -8526,9 +8520,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -8950,9 +8944,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -8960,9 +8954,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1100">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Power [MW]</a:t>
@@ -8983,9 +8977,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -9012,9 +9006,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -9051,7 +9045,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -10186,522 +10180,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>baseline case</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$B$5:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$P$4:$P$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.3633893020423198</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.8882762932856396</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.7375244634637204</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.68834067938222</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EAA8-49EA-8E78-20510F16E023}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>optimised case</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$B$5:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>compOptGebradd!$Q$4:$Q$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.7580800347977501</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.5614172705416101</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.5117378544789304</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.4127158655455796</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EAA8-49EA-8E78-20510F16E023}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="521064656"/>
-        <c:axId val="521062416"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="521064656"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="5"/>
-          <c:min val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Turbine number</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="521062416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="521062416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="5"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1200">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="el-GR" sz="1200">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>β</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t> [</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1000" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>o</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="1200">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="521064656"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -10993,7 +10471,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11003,7 +10481,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11026,7 +10504,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -11045,12 +10523,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -11061,7 +10536,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -11075,7 +10550,7 @@
         </c:txPr>
         <c:crossAx val="533155920"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickMarkSkip val="1"/>
@@ -11111,7 +10586,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11121,7 +10596,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11129,14 +10604,14 @@
                   <a:t>Thrust</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                  <a:rPr lang="en-GB" sz="1400" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> coefficient</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1200">
+                <a:endParaRPr lang="en-GB" sz="1400">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -11157,7 +10632,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -11176,12 +10651,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -11192,7 +10664,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -11206,7 +10678,7 @@
         </c:txPr>
         <c:crossAx val="533159120"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
         <c:majorUnit val="2.0000000000000004E-2"/>
       </c:valAx>
       <c:valAx>
@@ -11225,7 +10697,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11235,7 +10707,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200">
+                  <a:rPr lang="en-GB" sz="1400">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
@@ -11243,14 +10715,14 @@
                   <a:t>Wind</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1200" baseline="0">
+                  <a:rPr lang="en-GB" sz="1400" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t> speed [m/s]</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1200">
+                <a:endParaRPr lang="en-GB" sz="1400">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -11271,7 +10743,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
@@ -11306,7 +10778,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -11434,11 +10906,11 @@
           <c:x val="0.13963938728431022"/>
           <c:y val="3.5795161959565003E-2"/>
           <c:w val="0.75204137578766239"/>
-          <c:h val="0.62096019247764966"/>
+          <c:h val="0.68895221553391894"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -11447,7 +10919,7 @@
             <c:v>Turbine 1 - Literature</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -11507,7 +10979,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-46E5-4FA0-BFB0-ED6E8444DDB9}"/>
@@ -11521,7 +10993,7 @@
             <c:v>Turbine 1 - FASTnAT</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -11581,7 +11053,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-46E5-4FA0-BFB0-ED6E8444DDB9}"/>
@@ -11595,7 +11067,7 @@
             <c:v>Total - Literature</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -11654,7 +11126,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-800D-497D-8A0B-3DD9FE94C0F7}"/>
@@ -11668,7 +11140,7 @@
             <c:v>Turbine 2 - Literature</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="44450" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -11728,7 +11200,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-46E5-4FA0-BFB0-ED6E8444DDB9}"/>
@@ -11742,7 +11214,7 @@
             <c:v>Turbine 2 - FASTnAT</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="44450" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -11802,7 +11274,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-46E5-4FA0-BFB0-ED6E8444DDB9}"/>
@@ -11816,7 +11288,7 @@
             <c:v>Total - FASTnAT</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -11875,7 +11347,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-800D-497D-8A0B-3DD9FE94C0F7}"/>
@@ -11923,12 +11395,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -11936,14 +11405,42 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:rPr lang="en-GB" sz="1800">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Pitch</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
-                  <a:t> offset turbine 1 [deg]</a:t>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> offset turbine 1 [</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1600"/>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" baseline="30000">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>o</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -11960,12 +11457,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -11982,12 +11476,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -12000,10 +11491,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -12048,12 +11536,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -12061,14 +11546,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600"/>
+                  <a:rPr lang="en-GB" sz="1800">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Turbine</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1800" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t> power [MW]</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB" sz="1600"/>
+                <a:endParaRPr lang="en-GB" sz="1800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -12085,12 +11582,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -12107,12 +11601,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -12125,10 +11616,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -12153,16 +11641,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.421963684005679E-3"/>
-          <c:y val="0.79023952535830244"/>
-          <c:w val="0.99255903260169043"/>
-          <c:h val="0.20976033922496518"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12176,12 +11654,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -12204,9 +11679,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -14329,12 +13802,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -14444,12 +13914,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -17093,46 +16560,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors21.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -24108,522 +23535,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -28307,13 +27218,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>401653</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>162370</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>444381</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25638</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28849,15 +27760,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>205095</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>119642</xdr:rowOff>
+      <xdr:colOff>51274</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>17093</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>205099</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>119641</xdr:rowOff>
+      <xdr:colOff>606751</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>59821</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28885,15 +27796,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>8544</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>128187</xdr:rowOff>
+      <xdr:colOff>606750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>17091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>25637</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>119642</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>188007</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>102549</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28951,44 +27862,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>34183</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>153824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>34187</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>119640</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{884EACAC-D669-462D-8446-5954E9DDBAAD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -30294,7 +29167,7 @@
   <dimension ref="B2:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -30763,7 +29636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{309239CC-BC38-44E3-8E08-89E4685D5CB7}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -31358,7 +30231,7 @@
   <dimension ref="C2:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -34119,8 +32992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A1701E-EF5B-427E-BB04-C2713A8A8E89}">
   <dimension ref="B2:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -34480,7 +33353,7 @@
   <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>

</xml_diff>